<commit_message>
maj code carte arrière
</commit_message>
<xml_diff>
--- a/EL_Electrical/Faisceau/Récap connections.xlsx
+++ b/EL_Electrical/Faisceau/Récap connections.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7590" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Faisceau Avant" sheetId="1" r:id="rId1"/>
+    <sheet name="Faisceau Arrière" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -84,8 +85,118 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>bob Aubouin</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bob Aubouin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tout les capteurs du faisceau avant
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bob Aubouin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tout les capteurs du faisceau avant
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bob Aubouin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tout les capteurs du faisceau avant
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bob Aubouin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tout les capteurs du faisceau avant
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="91">
   <si>
     <t>Pare feu</t>
   </si>
@@ -226,6 +337,138 @@
   </si>
   <si>
     <t>Carte avant</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>shift cut</t>
+  </si>
+  <si>
+    <t>gearpot</t>
+  </si>
+  <si>
+    <t>wet/dry</t>
+  </si>
+  <si>
+    <t>Traction</t>
+  </si>
+  <si>
+    <t>Launch</t>
+  </si>
+  <si>
+    <t>log dta</t>
+  </si>
+  <si>
+    <t>RR ws</t>
+  </si>
+  <si>
+    <t>FR ws</t>
+  </si>
+  <si>
+    <t>FL ws</t>
+  </si>
+  <si>
+    <t>arbre à cam</t>
+  </si>
+  <si>
+    <t>cranckshaft</t>
+  </si>
+  <si>
+    <t>Twater</t>
+  </si>
+  <si>
+    <t>Tair</t>
+  </si>
+  <si>
+    <t>Pair</t>
+  </si>
+  <si>
+    <t>oil pressur</t>
+  </si>
+  <si>
+    <t>fuel pressur</t>
+  </si>
+  <si>
+    <t>5V capteurs</t>
+  </si>
+  <si>
+    <t>Masse DTA</t>
+  </si>
+  <si>
+    <t>DTA sensor</t>
+  </si>
+  <si>
+    <t>Masse cam+vilbrequin</t>
+  </si>
+  <si>
+    <t>DTA power</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>relais pompe</t>
+  </si>
+  <si>
+    <t>relais ventilo</t>
+  </si>
+  <si>
+    <t>inj1</t>
+  </si>
+  <si>
+    <t>inj2</t>
+  </si>
+  <si>
+    <t>inj3</t>
+  </si>
+  <si>
+    <t>inj4</t>
+  </si>
+  <si>
+    <t>spark1</t>
+  </si>
+  <si>
+    <t>spark2</t>
+  </si>
+  <si>
+    <t>spark3</t>
+  </si>
+  <si>
+    <t>spark4</t>
+  </si>
+  <si>
+    <t>5V MK3</t>
+  </si>
+  <si>
+    <t>Power Box</t>
+  </si>
+  <si>
+    <t>12V Masterswitch</t>
+  </si>
+  <si>
+    <t>12V Pompe</t>
+  </si>
+  <si>
+    <t>12V ventilo</t>
+  </si>
+  <si>
+    <t>12V Motored</t>
+  </si>
+  <si>
+    <t>12V Brake light</t>
+  </si>
+  <si>
+    <t>Command pomp</t>
+  </si>
+  <si>
+    <t>Command Ventilo</t>
+  </si>
+  <si>
+    <t>12V Gearbox controller</t>
+  </si>
+  <si>
+    <t>Démarreur</t>
   </si>
 </sst>
 </file>
@@ -371,17 +614,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -395,6 +629,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,477 +934,1128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
+      <c r="I1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
-      <c r="M1" s="1" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="16"/>
+      <c r="M1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="3"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="E3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="I3" s="7" t="s">
+      <c r="F3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="I3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="9"/>
-      <c r="M3" s="7" t="s">
+      <c r="J3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="M3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="9"/>
+      <c r="N3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="I4" s="7" t="s">
+      <c r="G4" s="6"/>
+      <c r="I4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="M4" s="7" t="s">
+      <c r="J4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="M4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" s="9"/>
+      <c r="N4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="E5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="I5" s="7" t="s">
+      <c r="F5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="M5" s="11" t="s">
+      <c r="K5" s="6"/>
+      <c r="M5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5" s="13"/>
+      <c r="N5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="E6" s="15" t="s">
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="E6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="I6" s="7" t="s">
+      <c r="F6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="I6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="9"/>
+      <c r="J6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="E7" s="16" t="s">
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="E7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="I7" s="7" t="s">
+      <c r="G7" s="10"/>
+      <c r="I7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="9"/>
-      <c r="M7" s="1" t="s">
+      <c r="J7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="M7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="3"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="I8" s="7" t="s">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="I8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="9"/>
-      <c r="M8" s="4" t="s">
+      <c r="J8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="M8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="I9" s="11" t="s">
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="I9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="M9" s="7" t="s">
+      <c r="J9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="M9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="O9" s="9"/>
+      <c r="N9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="M10" s="7" t="s">
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="M10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="9"/>
+      <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="E11" s="1" t="s">
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="E11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="1" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="I11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="7" t="s">
+      <c r="J11" s="15"/>
+      <c r="K11" s="16"/>
+      <c r="M11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="O11" s="9"/>
+      <c r="N11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="E12" s="4" t="s">
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="N12" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="O12" s="13"/>
+      <c r="N12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" s="10"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="E13" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="E13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="I13" s="7" t="s">
+      <c r="F13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="I13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="9"/>
+      <c r="J13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="E14" s="7" t="s">
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="E14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="I14" s="7" t="s">
+      <c r="G14" s="6"/>
+      <c r="I14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="9"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="E15" s="11" t="s">
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="E15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="I15" s="7" t="s">
+      <c r="F15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="I15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="9"/>
+      <c r="J15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="I16" s="15" t="s">
+      <c r="B16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="I16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="9"/>
+      <c r="J16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="I17" s="7" t="s">
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="I17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="9"/>
+      <c r="J17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="I18" s="11" t="s">
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="I18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="13"/>
+      <c r="J18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="M7:O7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
+      <c r="I1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="K1" s="16"/>
+      <c r="M1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="15"/>
+      <c r="O1" s="16"/>
+      <c r="Q1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" s="15"/>
+      <c r="S1" s="16"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="I3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="Q3" t="s">
+        <v>82</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="E4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="I4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="M4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="Q4" t="s">
+        <v>83</v>
+      </c>
+      <c r="R4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="E5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="I5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="M5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="Q5" t="s">
+        <v>84</v>
+      </c>
+      <c r="R5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="M6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="Q6" t="s">
+        <v>85</v>
+      </c>
+      <c r="R6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="I7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="M7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="Q7" t="s">
+        <v>86</v>
+      </c>
+      <c r="R7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="I8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="M8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="Q8" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="I9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="M9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="Q9" t="s">
+        <v>87</v>
+      </c>
+      <c r="R9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="I10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="M10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="Q10" t="s">
+        <v>88</v>
+      </c>
+      <c r="R10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="I11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="M11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="Q11" t="s">
+        <v>89</v>
+      </c>
+      <c r="R11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="I12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="M12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="I13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="M13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="I14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="M14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="I15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="I16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="I17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="I18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="I19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="I20" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="I21" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I24" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I25" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="Q1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
maj excel integration faisceau
</commit_message>
<xml_diff>
--- a/EL_Electrical/Faisceau/Récap connections.xlsx
+++ b/EL_Electrical/Faisceau/Récap connections.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobau\Documents\EPSA\Ressources2020\EL_Electrical\Faisceau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lecoc\Desktop\EPSA\Ressource 2020\EL_Electrical\Faisceau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7590" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20436" windowHeight="7596" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Faisceau Avant" sheetId="1" r:id="rId1"/>
     <sheet name="Faisceau Arrière" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -191,12 +191,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="E7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bob Aubouin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tout les capteurs du faisceau avant
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="99">
   <si>
     <t>Pare feu</t>
   </si>
@@ -469,12 +494,36 @@
   </si>
   <si>
     <t>Démarreur</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Capteurs pression d'huile</t>
+  </si>
+  <si>
+    <t>noir</t>
+  </si>
+  <si>
+    <t>vert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -629,6 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,7 +688,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,41 +970,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="E1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
-      <c r="I1" s="14" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="I1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
-      <c r="M1" s="14" t="s">
+      <c r="J1" s="16"/>
+      <c r="K1" s="17"/>
+      <c r="M1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="16"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -993,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1007,7 +1056,9 @@
       <c r="F3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="I3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1023,7 +1074,7 @@
       </c>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1037,7 +1088,9 @@
       <c r="F4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="I4" s="4" t="s">
         <v>33</v>
       </c>
@@ -1053,7 +1106,7 @@
       </c>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1067,7 +1120,9 @@
       <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1083,7 +1138,7 @@
       </c>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1152,9 @@
       <c r="F6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="I6" s="4" t="s">
         <v>34</v>
       </c>
@@ -1106,7 +1163,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1120,7 +1177,9 @@
       <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="I7" s="4" t="s">
         <v>35</v>
       </c>
@@ -1128,13 +1187,13 @@
         <v>16</v>
       </c>
       <c r="K7" s="6"/>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="16"/>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1159,7 +1218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1182,7 +1241,7 @@
       </c>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1198,7 +1257,7 @@
       </c>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1206,16 +1265,16 @@
         <v>16</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-      <c r="I11" s="14" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="I11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
       <c r="M11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1224,7 +1283,7 @@
       </c>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>44</v>
       </c>
@@ -1258,7 +1317,7 @@
       </c>
       <c r="O12" s="10"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1272,7 +1331,9 @@
       <c r="F13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6">
+        <v>3</v>
+      </c>
       <c r="I13" s="4" t="s">
         <v>27</v>
       </c>
@@ -1281,7 +1342,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1295,7 +1356,9 @@
       <c r="F14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="6">
+        <v>2</v>
+      </c>
       <c r="I14" s="4" t="s">
         <v>28</v>
       </c>
@@ -1304,7 +1367,7 @@
       </c>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -1318,7 +1381,9 @@
       <c r="F15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="10">
+        <v>1</v>
+      </c>
       <c r="I15" s="4" t="s">
         <v>17</v>
       </c>
@@ -1327,7 +1392,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -1343,7 +1408,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1359,7 +1424,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1375,7 +1440,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1384,7 +1449,7 @@
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1393,7 +1458,7 @@
       </c>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>80</v>
       </c>
@@ -1402,7 +1467,7 @@
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
@@ -1411,11 +1476,11 @@
       </c>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="10"/>
@@ -1441,48 +1506,48 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="25.7109375" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" customWidth="1"/>
+    <col min="17" max="17" width="25.6640625" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="E1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
-      <c r="I1" s="14" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="I1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
-      <c r="M1" s="14" t="s">
+      <c r="J1" s="16"/>
+      <c r="K1" s="17"/>
+      <c r="M1" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="16"/>
-      <c r="Q1" s="14" t="s">
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
+      <c r="Q1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="R1" s="15"/>
-      <c r="S1" s="16"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R1" s="16"/>
+      <c r="S1" s="17"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1529,7 +1594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1543,7 +1608,9 @@
       <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="6">
+        <v>3</v>
+      </c>
       <c r="I3" s="4" t="s">
         <v>47</v>
       </c>
@@ -1563,7 +1630,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1577,7 +1644,9 @@
       <c r="F4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6">
+        <v>2</v>
+      </c>
       <c r="I4" s="4" t="s">
         <v>48</v>
       </c>
@@ -1599,7 +1668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1613,7 +1682,9 @@
       <c r="F5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
       <c r="I5" s="4" t="s">
         <v>49</v>
       </c>
@@ -1635,7 +1706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1664,7 +1735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1672,6 +1743,11 @@
         <v>10</v>
       </c>
       <c r="C7" s="6"/>
+      <c r="E7" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
       <c r="I7" s="4" t="s">
         <v>51</v>
       </c>
@@ -1693,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1701,6 +1777,15 @@
         <v>5</v>
       </c>
       <c r="C8" s="6"/>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="I8" s="4" t="s">
         <v>52</v>
       </c>
@@ -1722,7 +1807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1730,6 +1815,15 @@
         <v>7</v>
       </c>
       <c r="C9" s="6"/>
+      <c r="E9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
       <c r="I9" s="4" t="s">
         <v>53</v>
       </c>
@@ -1751,7 +1845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1759,6 +1853,15 @@
         <v>16</v>
       </c>
       <c r="C10" s="6"/>
+      <c r="E10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="6">
+        <v>3</v>
+      </c>
       <c r="I10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1780,7 +1883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1788,6 +1891,15 @@
         <v>16</v>
       </c>
       <c r="C11" s="6"/>
+      <c r="E11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2</v>
+      </c>
       <c r="I11" s="4" t="s">
         <v>6</v>
       </c>
@@ -1809,7 +1921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>44</v>
       </c>
@@ -1832,7 +1944,7 @@
       </c>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1855,7 +1967,7 @@
       </c>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1873,12 +1985,12 @@
       <c r="M14" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="14" t="s">
         <v>25</v>
       </c>
       <c r="O14" s="10"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -1894,7 +2006,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -1910,7 +2022,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1926,7 +2038,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1942,7 +2054,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1958,7 +2070,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>80</v>
       </c>
@@ -1974,7 +2086,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1990,7 +2102,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
@@ -2005,7 +2117,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>90</v>
       </c>
@@ -2020,7 +2132,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I24" s="12" t="s">
         <v>63</v>
       </c>
@@ -2029,7 +2141,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I25" s="12" t="s">
         <v>64</v>
       </c>
@@ -2038,7 +2150,7 @@
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I26" s="13" t="s">
         <v>65</v>
       </c>
@@ -2048,7 +2160,8 @@
       <c r="K26" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="E7:G7"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="I1:K1"/>

</xml_diff>